<commit_message>
Add results for Test 2b
</commit_message>
<xml_diff>
--- a/results/hub_benchmarks.xlsx
+++ b/results/hub_benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\niva-of5\osl-userdata$\JES\System\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156191C1-775B-4841-BB2B-2FBA623E9B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83B7254-F38C-4499-972B-AC8D6B382C26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{38522D97-2D01-434E-9855-A549EF88FE11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{38522D97-2D01-434E-9855-A549EF88FE11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,13 +105,13 @@
     <t>Read and decompress 1 GB GeoTiff from shared disk (norway_kartverket_40m_dtm_utm_z33.tif)</t>
   </si>
   <si>
-    <t>Read and decompress 14 GB GeoTiff from shared disk (norway_kartverket_10m_dtm_utm_z33.tif). 64 GB machine</t>
-  </si>
-  <si>
     <t>Read 14 GB GeoTiff from shared (s)</t>
   </si>
   <si>
     <t>Read 1 GB GeoTiff from shared (s)</t>
+  </si>
+  <si>
+    <t>Read and decompress 14 GB GeoTiff from shared disk (norway_kartverket_10m_dtm_utm_z33.tif). 240 GB machine</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
   <dimension ref="A1:F161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E92" sqref="E92"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +493,7 @@
     <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="103.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="104.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2921,7 +2921,7 @@
         <v>19</v>
       </c>
       <c r="B122" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -2941,7 +2941,7 @@
         <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C123">
         <v>2</v>
@@ -2961,7 +2961,7 @@
         <v>19</v>
       </c>
       <c r="B124" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C124">
         <v>3</v>
@@ -2981,7 +2981,7 @@
         <v>19</v>
       </c>
       <c r="B125" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C125">
         <v>4</v>
@@ -3001,7 +3001,7 @@
         <v>19</v>
       </c>
       <c r="B126" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C126">
         <v>5</v>
@@ -3021,7 +3021,7 @@
         <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C127">
         <v>6</v>
@@ -3041,7 +3041,7 @@
         <v>19</v>
       </c>
       <c r="B128" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C128">
         <v>7</v>
@@ -3061,7 +3061,7 @@
         <v>19</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C129">
         <v>8</v>
@@ -3081,7 +3081,7 @@
         <v>19</v>
       </c>
       <c r="B130" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C130">
         <v>9</v>
@@ -3101,7 +3101,7 @@
         <v>19</v>
       </c>
       <c r="B131" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C131">
         <v>10</v>
@@ -3121,7 +3121,7 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -3141,7 +3141,7 @@
         <v>19</v>
       </c>
       <c r="B133" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C133">
         <v>2</v>
@@ -3161,7 +3161,7 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C134">
         <v>3</v>
@@ -3181,7 +3181,7 @@
         <v>19</v>
       </c>
       <c r="B135" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C135">
         <v>4</v>
@@ -3201,7 +3201,7 @@
         <v>19</v>
       </c>
       <c r="B136" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C136">
         <v>5</v>
@@ -3221,7 +3221,7 @@
         <v>19</v>
       </c>
       <c r="B137" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C137">
         <v>6</v>
@@ -3241,7 +3241,7 @@
         <v>19</v>
       </c>
       <c r="B138" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C138">
         <v>7</v>
@@ -3261,7 +3261,7 @@
         <v>19</v>
       </c>
       <c r="B139" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C139">
         <v>8</v>
@@ -3281,7 +3281,7 @@
         <v>19</v>
       </c>
       <c r="B140" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C140">
         <v>9</v>
@@ -3301,7 +3301,7 @@
         <v>19</v>
       </c>
       <c r="B141" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C141">
         <v>10</v>
@@ -3321,7 +3321,7 @@
         <v>20</v>
       </c>
       <c r="B142" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -3333,7 +3333,7 @@
         <v>177.9</v>
       </c>
       <c r="F142" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -3341,7 +3341,7 @@
         <v>20</v>
       </c>
       <c r="B143" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C143">
         <v>2</v>
@@ -3353,7 +3353,7 @@
         <v>170.9</v>
       </c>
       <c r="F143" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -3361,7 +3361,7 @@
         <v>20</v>
       </c>
       <c r="B144" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C144">
         <v>3</v>
@@ -3373,7 +3373,7 @@
         <v>171.8</v>
       </c>
       <c r="F144" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -3381,7 +3381,7 @@
         <v>20</v>
       </c>
       <c r="B145" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C145">
         <v>4</v>
@@ -3393,7 +3393,7 @@
         <v>170.9</v>
       </c>
       <c r="F145" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
         <v>20</v>
       </c>
       <c r="B146" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C146">
         <v>5</v>
@@ -3413,7 +3413,7 @@
         <v>171.2</v>
       </c>
       <c r="F146" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -3421,7 +3421,7 @@
         <v>20</v>
       </c>
       <c r="B147" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C147">
         <v>6</v>
@@ -3433,7 +3433,7 @@
         <v>171.3</v>
       </c>
       <c r="F147" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -3441,7 +3441,7 @@
         <v>20</v>
       </c>
       <c r="B148" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C148">
         <v>7</v>
@@ -3453,7 +3453,7 @@
         <v>171.4</v>
       </c>
       <c r="F148" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -3461,7 +3461,7 @@
         <v>20</v>
       </c>
       <c r="B149" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C149">
         <v>8</v>
@@ -3473,7 +3473,7 @@
         <v>171.8</v>
       </c>
       <c r="F149" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -3481,7 +3481,7 @@
         <v>20</v>
       </c>
       <c r="B150" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C150">
         <v>9</v>
@@ -3493,7 +3493,7 @@
         <v>171.1</v>
       </c>
       <c r="F150" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -3501,7 +3501,7 @@
         <v>20</v>
       </c>
       <c r="B151" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C151">
         <v>10</v>
@@ -3513,7 +3513,7 @@
         <v>171.9</v>
       </c>
       <c r="F151" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -3521,7 +3521,7 @@
         <v>20</v>
       </c>
       <c r="B152" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -3529,8 +3529,11 @@
       <c r="D152" t="s">
         <v>6</v>
       </c>
+      <c r="E152">
+        <v>191.6</v>
+      </c>
       <c r="F152" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -3538,7 +3541,7 @@
         <v>20</v>
       </c>
       <c r="B153" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C153">
         <v>2</v>
@@ -3546,8 +3549,11 @@
       <c r="D153" t="s">
         <v>6</v>
       </c>
+      <c r="E153">
+        <v>183.4</v>
+      </c>
       <c r="F153" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -3555,7 +3561,7 @@
         <v>20</v>
       </c>
       <c r="B154" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C154">
         <v>3</v>
@@ -3563,8 +3569,11 @@
       <c r="D154" t="s">
         <v>6</v>
       </c>
+      <c r="E154">
+        <v>184.1</v>
+      </c>
       <c r="F154" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -3572,7 +3581,7 @@
         <v>20</v>
       </c>
       <c r="B155" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C155">
         <v>4</v>
@@ -3580,8 +3589,11 @@
       <c r="D155" t="s">
         <v>6</v>
       </c>
+      <c r="E155">
+        <v>183.3</v>
+      </c>
       <c r="F155" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -3589,7 +3601,7 @@
         <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C156">
         <v>5</v>
@@ -3597,8 +3609,11 @@
       <c r="D156" t="s">
         <v>6</v>
       </c>
+      <c r="E156">
+        <v>183.5</v>
+      </c>
       <c r="F156" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -3606,7 +3621,7 @@
         <v>20</v>
       </c>
       <c r="B157" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C157">
         <v>6</v>
@@ -3614,8 +3629,11 @@
       <c r="D157" t="s">
         <v>6</v>
       </c>
+      <c r="E157">
+        <v>184</v>
+      </c>
       <c r="F157" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -3623,7 +3641,7 @@
         <v>20</v>
       </c>
       <c r="B158" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C158">
         <v>7</v>
@@ -3631,8 +3649,11 @@
       <c r="D158" t="s">
         <v>6</v>
       </c>
+      <c r="E158">
+        <v>183.9</v>
+      </c>
       <c r="F158" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -3640,7 +3661,7 @@
         <v>20</v>
       </c>
       <c r="B159" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C159">
         <v>8</v>
@@ -3648,8 +3669,11 @@
       <c r="D159" t="s">
         <v>6</v>
       </c>
+      <c r="E159">
+        <v>184.2</v>
+      </c>
       <c r="F159" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -3657,7 +3681,7 @@
         <v>20</v>
       </c>
       <c r="B160" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C160">
         <v>9</v>
@@ -3665,8 +3689,11 @@
       <c r="D160" t="s">
         <v>6</v>
       </c>
+      <c r="E160">
+        <v>184.8</v>
+      </c>
       <c r="F160" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -3674,7 +3701,7 @@
         <v>20</v>
       </c>
       <c r="B161" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C161">
         <v>10</v>
@@ -3682,8 +3709,11 @@
       <c r="D161" t="s">
         <v>6</v>
       </c>
+      <c r="E161">
+        <v>184.8</v>
+      </c>
       <c r="F161" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>